<commit_message>
Added TestingDocument and Updated Testing Doucments
</commit_message>
<xml_diff>
--- a/reportsAndLogs/Reports/TestCase_000.xlsx
+++ b/reportsAndLogs/Reports/TestCase_000.xlsx
@@ -137,10 +137,10 @@
     <t>The username password windows should be opened</t>
   </si>
   <si>
-    <t>The login whould be successful</t>
-  </si>
-  <si>
     <t>Enter username and password and click login button</t>
+  </si>
+  <si>
+    <t>The login would be successful</t>
   </si>
 </sst>
 </file>
@@ -150,7 +150,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +188,22 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -288,9 +304,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -332,20 +350,52 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -360,50 +410,20 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
@@ -720,23 +740,23 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="16"/>
       <c r="C1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="25"/>
+      <c r="E1" s="16"/>
       <c r="F1" s="17" t="s">
         <v>29</v>
       </c>
@@ -747,27 +767,27 @@
       <c r="K1" s="18"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="25"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="17"/>
       <c r="G2" s="18"/>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="37" t="s">
+      <c r="I2" s="16"/>
+      <c r="J2" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="38"/>
+      <c r="K2" s="21"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
@@ -783,10 +803,10 @@
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="32"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -811,29 +831,29 @@
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="34" t="s">
+      <c r="E6" s="23"/>
+      <c r="F6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="H6" s="33" t="s">
+      <c r="G6" s="25"/>
+      <c r="H6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="36" t="s">
+      <c r="I6" s="23"/>
+      <c r="J6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="36"/>
+      <c r="K6" s="14"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
@@ -852,28 +872,28 @@
       <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="8"/>
       <c r="F8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>1</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="29" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="17"/>
@@ -882,7 +902,7 @@
       <c r="F9" s="9">
         <v>1</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="29" t="s">
         <v>25</v>
       </c>
       <c r="H9" s="17"/>
@@ -894,14 +914,14 @@
       <c r="A10" s="9">
         <v>2</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="17"/>
       <c r="D10" s="18"/>
       <c r="E10" s="2"/>
       <c r="F10" s="9">
         <v>2</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="29" t="s">
         <v>26</v>
       </c>
       <c r="H10" s="17"/>
@@ -913,14 +933,14 @@
       <c r="A11" s="9">
         <v>3</v>
       </c>
-      <c r="B11" s="16"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="17"/>
       <c r="D11" s="18"/>
       <c r="E11" s="2"/>
       <c r="F11" s="9">
         <v>3</v>
       </c>
-      <c r="G11" s="16"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
@@ -930,14 +950,14 @@
       <c r="A12" s="9">
         <v>4</v>
       </c>
-      <c r="B12" s="16"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="17"/>
       <c r="D12" s="18"/>
       <c r="E12" s="2"/>
       <c r="F12" s="9">
         <v>4</v>
       </c>
-      <c r="G12" s="16"/>
+      <c r="G12" s="29"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
@@ -987,59 +1007,59 @@
       <c r="K15" s="10"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="23" t="s">
+      <c r="C16" s="31"/>
+      <c r="D16" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="20" t="s">
+      <c r="E16" s="34"/>
+      <c r="F16" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="20" t="s">
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
     </row>
     <row r="18" spans="1:11" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>1</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="14" t="s">
+      <c r="C18" s="37"/>
+      <c r="D18" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="16" t="s">
+      <c r="E18" s="36"/>
+      <c r="F18" s="29" t="s">
         <v>21</v>
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="18"/>
-      <c r="I18" s="16" t="s">
+      <c r="I18" s="29" t="s">
         <v>9</v>
       </c>
       <c r="J18" s="17"/>
@@ -1049,20 +1069,20 @@
       <c r="A19" s="9">
         <v>2</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="14" t="s">
+      <c r="C19" s="38"/>
+      <c r="D19" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="16" t="s">
+      <c r="E19" s="36"/>
+      <c r="F19" s="29" t="s">
         <v>21</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="18"/>
-      <c r="I19" s="16" t="s">
+      <c r="I19" s="29" t="s">
         <v>9</v>
       </c>
       <c r="J19" s="17"/>
@@ -1072,20 +1092,20 @@
       <c r="A20" s="9">
         <v>3</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="14" t="s">
+      <c r="C20" s="38"/>
+      <c r="D20" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="16" t="s">
+      <c r="E20" s="38"/>
+      <c r="F20" s="29" t="s">
         <v>21</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="18"/>
-      <c r="I20" s="16" t="s">
+      <c r="I20" s="29" t="s">
         <v>9</v>
       </c>
       <c r="J20" s="17"/>
@@ -1095,20 +1115,20 @@
       <c r="A21" s="9">
         <v>4</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="38"/>
+      <c r="D21" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="16" t="s">
+      <c r="E21" s="38"/>
+      <c r="F21" s="29" t="s">
         <v>21</v>
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="18"/>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="29" t="s">
         <v>9</v>
       </c>
       <c r="J21" s="17"/>
@@ -1116,32 +1136,71 @@
     </row>
     <row r="22" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="16"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="29"/>
       <c r="G22" s="17"/>
       <c r="H22" s="18"/>
-      <c r="I22" s="16"/>
+      <c r="I22" s="29"/>
       <c r="J22" s="17"/>
       <c r="K22" s="18"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="16"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="29"/>
       <c r="G23" s="17"/>
       <c r="H23" s="18"/>
-      <c r="I23" s="16"/>
+      <c r="I23" s="29"/>
       <c r="J23" s="17"/>
       <c r="K23" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="I16:K17"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
@@ -1156,45 +1215,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="F16:H17"/>
-    <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:K23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>